<commit_message>
Updated inputs including umya and rust version. json is sorted before typst gets it.
</commit_message>
<xml_diff>
--- a/package/Book.xlsx
+++ b/package/Book.xlsx
@@ -69,7 +69,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -78,26 +78,104 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor rgb="FFFFC000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="5"/>
-        <bgColor indexed="5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="2"/>
-        <bgColor indexed="2"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCFA219"/>
-        <bgColor rgb="FFCFA219"/>
+        <fgColor theme="0" tint="-0.049989318521683403"/>
+        <bgColor theme="0" tint="-0.049989318521683403"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor theme="1" tint="0.499984740745262"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.099978637043366805"/>
+        <bgColor theme="2" tint="-0.099978637043366805"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor theme="3" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.34998626667073579"/>
+        <bgColor theme="1" tint="0.34998626667073579"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor theme="2" tint="-0.249977111117893"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor theme="3" tint="0.39997558519241921"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor theme="0" tint="-0.249977111117893"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.249977111117893"/>
+        <bgColor theme="1" tint="0.249977111117893"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor theme="7" tint="0.39997558519241921"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor theme="9" tint="0.39997558519241921"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.499984740745262"/>
+        <bgColor theme="2" tint="-0.499984740745262"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor theme="5" tint="-0.249977111117893"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor rgb="FF00B050"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0"/>
+        <bgColor theme="7" tint="0"/>
       </patternFill>
     </fill>
   </fills>
@@ -197,48 +275,53 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="20">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="2" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf fontId="0" fillId="3" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="4" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="2" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="5" borderId="2" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="6" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf fontId="0" fillId="7" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf fontId="0" fillId="2" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="8" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="2" borderId="3" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="8" borderId="3" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+    <xf fontId="0" fillId="9" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="0" fillId="3" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="10" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf fontId="0" fillId="11" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="0" fillId="4" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="12" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf fontId="0" fillId="5" borderId="4" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="10" borderId="4" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="5" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="13" borderId="5" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="14" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf fontId="0" fillId="15" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf fontId="0" fillId="16" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="6" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="17" borderId="6" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf fontId="0" fillId="18" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -772,45 +855,48 @@
       <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="5"/>
     </row>
     <row r="2" ht="31.199999999999999" customHeight="1">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="8" t="s">
+      <c r="C2" s="8"/>
+      <c r="D2" s="9" t="s">
         <v>6</v>
       </c>
+      <c r="E2" s="10"/>
     </row>
     <row r="3" ht="38.399999999999999" customHeight="1">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="15" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" ht="86.25" customHeight="1">
-      <c r="A4" s="9"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="13" t="s">
+      <c r="A4" s="11"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="18" t="s">
         <v>13</v>
       </c>
+      <c r="E4" s="19"/>
     </row>
     <row r="14" ht="14.25"/>
   </sheetData>

</xml_diff>